<commit_message>
Cargue de tablas y visualización con niveles de Jerarquía (en Fecha)
</commit_message>
<xml_diff>
--- a/4. Proyecto Finanzas Personales/Finanzas.xlsx
+++ b/4. Proyecto Finanzas Personales/Finanzas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Proyectos Power BI\Proyecto 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Udemy-s-Power-BI-Course\4. Proyecto Finanzas Personales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99558217-5CDB-4539-8680-CDA5314E853B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909FB5F4-CC81-4463-9C9C-68A1046647EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos" sheetId="11" r:id="rId1"/>
@@ -278,12 +278,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="164" formatCode="m/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,6 +566,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1178987-F45E-49E5-B00E-5F36CADA6B99}" name="TablaIngresos" displayName="TablaIngresos" ref="A3:C51" totalsRowShown="0">
+  <autoFilter ref="A3:C51" xr:uid="{A1178987-F45E-49E5-B00E-5F36CADA6B99}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{19A28D37-ED01-4B7D-9BAB-FF8C7B28D17A}" name="Categoria"/>
+    <tableColumn id="2" xr3:uid="{3EBEFD33-22A5-4FA1-947E-60D01541A991}" name="Fecha" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A8BC8C45-DC26-41AD-BC79-3600303414DD}" name="Cantidad"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaGastos" displayName="TablaGastos" ref="A3:C219" totalsRowShown="0">
   <autoFilter ref="A3:C219" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C217">
@@ -577,7 +592,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TablaMetas" displayName="TablaMetas" ref="A3:C27" totalsRowShown="0">
   <autoFilter ref="A3:C27" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
@@ -589,7 +604,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TablaPresupuesto" displayName="TablaPresupuesto" ref="A3:Y12" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:Y12" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -915,7 +930,7 @@
   <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,9 +993,6 @@
         <v>44166</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4">
         <v>10078</v>
       </c>
     </row>
@@ -992,9 +1004,6 @@
         <v>44166</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5">
         <v>13888</v>
       </c>
     </row>
@@ -1006,9 +1015,6 @@
         <v>44136</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="E6">
         <v>10002</v>
       </c>
     </row>
@@ -1514,6 +1520,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>